<commit_message>
changed type the days quiz
</commit_message>
<xml_diff>
--- a/Source Workbooks/Basic list copying and fill-ins.xlsx
+++ b/Source Workbooks/Basic list copying and fill-ins.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Desktop\HACC Laptop materials\Source Workbooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Desktop\Writing\ESLexercise.com\Source Workbooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5139F680-8501-4B3F-BE5A-952C325FC883}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDB454D4-31EA-42D3-866B-64A314E64D6C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,19 +25,11 @@
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Type the Months'!$A$4:$H$54</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="69">
   <si>
     <t>January</t>
   </si>
@@ -111,16 +103,10 @@
     <t>Español</t>
   </si>
   <si>
-    <t>Français:</t>
-  </si>
-  <si>
     <t>English:</t>
   </si>
   <si>
     <t>Copy :</t>
-  </si>
-  <si>
-    <t>TYPE THE DAYS</t>
   </si>
   <si>
     <t>TYPE THE MONTHS</t>
@@ -239,6 +225,18 @@
   <si>
     <t>sabado</t>
   </si>
+  <si>
+    <t>YouDo ESL</t>
+  </si>
+  <si>
+    <t>useHTTPS = "True"</t>
+  </si>
+  <si>
+    <t>ESLexercise.com/ Match the letters</t>
+  </si>
+  <si>
+    <t>Français</t>
+  </si>
 </sst>
 </file>
 
@@ -248,7 +246,7 @@
     <numFmt numFmtId="164" formatCode="_([$$-409]* #,##0.00_);_([$$-409]* \(#,##0.00\);_([$$-409]* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -333,6 +331,42 @@
       <name val="Bodoni MT"/>
       <family val="1"/>
     </font>
+    <font>
+      <sz val="24"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Comic Sans MS"/>
+      <family val="4"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -360,7 +394,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -429,15 +463,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -465,7 +490,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="77">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -574,17 +599,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
       <protection locked="0"/>
     </xf>
@@ -594,7 +619,7 @@
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -605,9 +630,6 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -627,194 +649,326 @@
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left"/>
-      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="289">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="5" tint="0.59996337778862885"/>
+  <dxfs count="305">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="5" tint="0.59996337778862885"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="3" tint="0.79998168889431442"/>
         </patternFill>
       </fill>
     </dxf>
@@ -2685,6 +2839,61 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>106681</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>230777</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1074421</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>186146</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{300BBC5D-CB21-46CB-89EF-A8B55DC29C31}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="716281" y="977537"/>
+          <a:ext cx="967740" cy="1418409"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -2692,6 +2901,7 @@
       <sheetName val="Sheet1"/>
     </sheetNames>
     <definedNames>
+      <definedName name="wwsImage"/>
       <definedName name="wwsInput"/>
       <definedName name="wwsSetup"/>
     </definedNames>
@@ -3047,7 +3257,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="13.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="str">
+      <c r="A1" s="60" t="str">
         <f>[1]!wwsSetup("useHTTPS", TRUE)</f>
         <v>useHTTPS = "True"</v>
       </c>
@@ -3066,7 +3276,7 @@
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="66" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B2" s="66"/>
       <c r="C2" s="66"/>
@@ -3082,20 +3292,20 @@
       <c r="M2" s="8"/>
     </row>
     <row r="3" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="68" t="str">
+      <c r="A3" s="65" t="str">
         <f>CONCATENATE("©ESLatHoward.com"," ","2/6/20")</f>
         <v>©ESLatHoward.com 2/6/20</v>
       </c>
-      <c r="B3" s="68"/>
-      <c r="C3" s="68"/>
-      <c r="D3" s="68"/>
-      <c r="E3" s="68"/>
-      <c r="F3" s="68"/>
-      <c r="G3" s="65"/>
+      <c r="B3" s="65"/>
+      <c r="C3" s="65"/>
+      <c r="D3" s="65"/>
+      <c r="E3" s="65"/>
+      <c r="F3" s="65"/>
+      <c r="G3" s="64"/>
       <c r="H3" s="11"/>
       <c r="I3" s="8"/>
       <c r="J3" s="25"/>
-      <c r="K3" s="65"/>
+      <c r="K3" s="64"/>
       <c r="L3" s="11"/>
       <c r="M3" s="8"/>
     </row>
@@ -3103,23 +3313,23 @@
       <c r="A4" s="23"/>
       <c r="B4" s="26"/>
       <c r="C4" s="40"/>
-      <c r="D4" s="64" t="s">
-        <v>26</v>
+      <c r="D4" s="63" t="s">
+        <v>25</v>
       </c>
       <c r="E4" s="28"/>
-      <c r="F4" s="62" t="s">
+      <c r="F4" s="61" t="s">
         <v>22</v>
       </c>
       <c r="G4" s="40"/>
-      <c r="H4" s="63" t="s">
-        <v>25</v>
-      </c>
-      <c r="J4" s="62" t="s">
+      <c r="H4" s="62" t="s">
+        <v>24</v>
+      </c>
+      <c r="J4" s="61" t="s">
         <v>23</v>
       </c>
       <c r="K4" s="40"/>
-      <c r="L4" s="63" t="s">
-        <v>25</v>
+      <c r="L4" s="62" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.7">
@@ -3137,7 +3347,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="G5" s="21"/>
       <c r="H5" s="35" t="str">
@@ -3149,7 +3359,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J5" s="21" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K5" s="21"/>
       <c r="L5" s="35" t="str">
@@ -3176,7 +3386,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="G6" s="30"/>
       <c r="H6" s="36" t="str">
@@ -3188,7 +3398,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J6" s="21" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="K6" s="30"/>
       <c r="L6" s="36" t="str">
@@ -3215,7 +3425,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="G7" s="21"/>
       <c r="H7" s="36" t="str">
@@ -3227,7 +3437,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J7" s="21" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="K7" s="21"/>
       <c r="L7" s="36" t="str">
@@ -3254,7 +3464,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G8" s="30"/>
       <c r="H8" s="36" t="str">
@@ -3266,7 +3476,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J8" s="21" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="K8" s="30"/>
       <c r="L8" s="36" t="str">
@@ -3293,7 +3503,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="G9" s="21"/>
       <c r="H9" s="36" t="str">
@@ -3305,7 +3515,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J9" s="21" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="K9" s="21"/>
       <c r="L9" s="36" t="str">
@@ -3332,7 +3542,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="G10" s="30"/>
       <c r="H10" s="36" t="str">
@@ -3344,7 +3554,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J10" s="21" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="K10" s="30"/>
       <c r="L10" s="36" t="str">
@@ -3371,7 +3581,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="G11" s="21"/>
       <c r="H11" s="36" t="str">
@@ -3383,7 +3593,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J11" s="21" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="K11" s="21"/>
       <c r="L11" s="36" t="str">
@@ -3410,7 +3620,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="G12" s="30"/>
       <c r="H12" s="36" t="str">
@@ -3422,7 +3632,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J12" s="21" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="K12" s="30"/>
       <c r="L12" s="36" t="str">
@@ -3449,7 +3659,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="G13" s="21"/>
       <c r="H13" s="36" t="str">
@@ -3461,7 +3671,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J13" s="21" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13" s="36" t="str">
@@ -3488,7 +3698,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F14" s="21" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G14" s="30"/>
       <c r="H14" s="36" t="str">
@@ -3500,7 +3710,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J14" s="21" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="K14" s="30"/>
       <c r="L14" s="36" t="str">
@@ -3527,7 +3737,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="G15" s="21"/>
       <c r="H15" s="36" t="str">
@@ -3539,7 +3749,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J15" s="21" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="K15" s="21"/>
       <c r="L15" s="36" t="str">
@@ -3566,7 +3776,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" s="30"/>
       <c r="H16" s="36" t="str">
@@ -3578,7 +3788,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="J16" s="21" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K16" s="30"/>
       <c r="L16" s="36" t="str">
@@ -4254,938 +4464,938 @@
     <mergeCell ref="A2:D2"/>
   </mergeCells>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="288" priority="440" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="287" priority="441" operator="equal">
+    <cfRule type="cellIs" dxfId="304" priority="440" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="303" priority="441" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="286" priority="439" operator="equal">
+    <cfRule type="cellIs" dxfId="302" priority="439" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="285" priority="518" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="284" priority="519" operator="equal">
+    <cfRule type="cellIs" dxfId="301" priority="518" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="300" priority="519" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E5">
-    <cfRule type="cellIs" dxfId="283" priority="517" operator="equal">
+    <cfRule type="cellIs" dxfId="299" priority="517" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="282" priority="410" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="281" priority="411" operator="equal">
+    <cfRule type="cellIs" dxfId="298" priority="410" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="297" priority="411" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="280" priority="409" operator="equal">
+    <cfRule type="cellIs" dxfId="296" priority="409" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="279" priority="431" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="278" priority="432" operator="equal">
+    <cfRule type="cellIs" dxfId="295" priority="431" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="294" priority="432" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="277" priority="430" operator="equal">
+    <cfRule type="cellIs" dxfId="293" priority="430" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="276" priority="428" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="275" priority="429" operator="equal">
+    <cfRule type="cellIs" dxfId="292" priority="428" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="291" priority="429" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E6">
-    <cfRule type="cellIs" dxfId="274" priority="427" operator="equal">
+    <cfRule type="cellIs" dxfId="290" priority="427" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="273" priority="422" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="272" priority="423" operator="equal">
+    <cfRule type="cellIs" dxfId="289" priority="422" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="288" priority="423" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="271" priority="421" operator="equal">
+    <cfRule type="cellIs" dxfId="287" priority="421" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="270" priority="425" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="269" priority="426" operator="equal">
+    <cfRule type="cellIs" dxfId="286" priority="425" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="285" priority="426" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E7">
-    <cfRule type="cellIs" dxfId="268" priority="424" operator="equal">
+    <cfRule type="cellIs" dxfId="284" priority="424" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="267" priority="416" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="266" priority="417" operator="equal">
+    <cfRule type="cellIs" dxfId="283" priority="416" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="282" priority="417" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="265" priority="415" operator="equal">
+    <cfRule type="cellIs" dxfId="281" priority="415" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="264" priority="419" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="263" priority="420" operator="equal">
+    <cfRule type="cellIs" dxfId="280" priority="419" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="279" priority="420" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E8">
-    <cfRule type="cellIs" dxfId="262" priority="418" operator="equal">
+    <cfRule type="cellIs" dxfId="278" priority="418" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="261" priority="413" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="260" priority="414" operator="equal">
+    <cfRule type="cellIs" dxfId="277" priority="413" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="276" priority="414" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E9">
-    <cfRule type="cellIs" dxfId="259" priority="412" operator="equal">
+    <cfRule type="cellIs" dxfId="275" priority="412" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="258" priority="404" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="257" priority="405" operator="equal">
+    <cfRule type="cellIs" dxfId="274" priority="404" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="273" priority="405" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="256" priority="403" operator="equal">
+    <cfRule type="cellIs" dxfId="272" priority="403" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="255" priority="407" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="254" priority="408" operator="equal">
+    <cfRule type="cellIs" dxfId="271" priority="407" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="270" priority="408" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E10">
-    <cfRule type="cellIs" dxfId="253" priority="406" operator="equal">
+    <cfRule type="cellIs" dxfId="269" priority="406" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="252" priority="398" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="251" priority="399" operator="equal">
+    <cfRule type="cellIs" dxfId="268" priority="398" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="267" priority="399" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="250" priority="397" operator="equal">
+    <cfRule type="cellIs" dxfId="266" priority="397" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="249" priority="401" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="248" priority="402" operator="equal">
+    <cfRule type="cellIs" dxfId="265" priority="401" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="264" priority="402" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E11">
-    <cfRule type="cellIs" dxfId="247" priority="400" operator="equal">
+    <cfRule type="cellIs" dxfId="263" priority="400" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="246" priority="392" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="245" priority="393" operator="equal">
+    <cfRule type="cellIs" dxfId="262" priority="392" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="261" priority="393" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="244" priority="391" operator="equal">
+    <cfRule type="cellIs" dxfId="260" priority="391" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="243" priority="395" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="242" priority="396" operator="equal">
+    <cfRule type="cellIs" dxfId="259" priority="395" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="258" priority="396" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E12">
-    <cfRule type="cellIs" dxfId="241" priority="394" operator="equal">
+    <cfRule type="cellIs" dxfId="257" priority="394" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="240" priority="386" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="239" priority="387" operator="equal">
+    <cfRule type="cellIs" dxfId="256" priority="386" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="255" priority="387" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="238" priority="385" operator="equal">
+    <cfRule type="cellIs" dxfId="254" priority="385" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="237" priority="389" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="236" priority="390" operator="equal">
+    <cfRule type="cellIs" dxfId="253" priority="389" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="252" priority="390" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E13">
-    <cfRule type="cellIs" dxfId="235" priority="388" operator="equal">
+    <cfRule type="cellIs" dxfId="251" priority="388" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="234" priority="380" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="233" priority="381" operator="equal">
+    <cfRule type="cellIs" dxfId="250" priority="380" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="249" priority="381" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="232" priority="379" operator="equal">
+    <cfRule type="cellIs" dxfId="248" priority="379" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="231" priority="383" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="230" priority="384" operator="equal">
+    <cfRule type="cellIs" dxfId="247" priority="383" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="246" priority="384" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E14">
-    <cfRule type="cellIs" dxfId="229" priority="382" operator="equal">
+    <cfRule type="cellIs" dxfId="245" priority="382" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="228" priority="374" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="227" priority="375" operator="equal">
+    <cfRule type="cellIs" dxfId="244" priority="374" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="243" priority="375" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="226" priority="373" operator="equal">
+    <cfRule type="cellIs" dxfId="242" priority="373" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="225" priority="377" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="224" priority="378" operator="equal">
+    <cfRule type="cellIs" dxfId="241" priority="377" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="240" priority="378" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E15">
-    <cfRule type="cellIs" dxfId="223" priority="376" operator="equal">
+    <cfRule type="cellIs" dxfId="239" priority="376" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="222" priority="368" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="221" priority="369" operator="equal">
+    <cfRule type="cellIs" dxfId="238" priority="368" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="237" priority="369" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="220" priority="367" operator="equal">
+    <cfRule type="cellIs" dxfId="236" priority="367" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="219" priority="371" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="218" priority="372" operator="equal">
+    <cfRule type="cellIs" dxfId="235" priority="371" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="234" priority="372" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E16">
-    <cfRule type="cellIs" dxfId="217" priority="370" operator="equal">
+    <cfRule type="cellIs" dxfId="233" priority="370" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="216" priority="194" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="215" priority="195" operator="equal">
+    <cfRule type="cellIs" dxfId="232" priority="194" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="231" priority="195" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="214" priority="193" operator="equal">
+    <cfRule type="cellIs" dxfId="230" priority="193" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="213" priority="215" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="212" priority="216" operator="equal">
+    <cfRule type="cellIs" dxfId="229" priority="215" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="228" priority="216" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="211" priority="214" operator="equal">
+    <cfRule type="cellIs" dxfId="227" priority="214" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="210" priority="212" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="209" priority="213" operator="equal">
+    <cfRule type="cellIs" dxfId="226" priority="212" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="225" priority="213" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I6">
-    <cfRule type="cellIs" dxfId="208" priority="211" operator="equal">
+    <cfRule type="cellIs" dxfId="224" priority="211" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="207" priority="206" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="206" priority="207" operator="equal">
+    <cfRule type="cellIs" dxfId="223" priority="206" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="222" priority="207" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="205" priority="205" operator="equal">
+    <cfRule type="cellIs" dxfId="221" priority="205" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="204" priority="209" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="203" priority="210" operator="equal">
+    <cfRule type="cellIs" dxfId="220" priority="209" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="219" priority="210" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I7">
-    <cfRule type="cellIs" dxfId="202" priority="208" operator="equal">
+    <cfRule type="cellIs" dxfId="218" priority="208" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="201" priority="200" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="200" priority="201" operator="equal">
+    <cfRule type="cellIs" dxfId="217" priority="200" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="216" priority="201" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="199" priority="199" operator="equal">
+    <cfRule type="cellIs" dxfId="215" priority="199" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="198" priority="203" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="197" priority="204" operator="equal">
+    <cfRule type="cellIs" dxfId="214" priority="203" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="213" priority="204" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I8">
-    <cfRule type="cellIs" dxfId="196" priority="202" operator="equal">
+    <cfRule type="cellIs" dxfId="212" priority="202" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="195" priority="197" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="194" priority="198" operator="equal">
+    <cfRule type="cellIs" dxfId="211" priority="197" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="210" priority="198" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9">
-    <cfRule type="cellIs" dxfId="193" priority="196" operator="equal">
+    <cfRule type="cellIs" dxfId="209" priority="196" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="192" priority="188" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="191" priority="189" operator="equal">
+    <cfRule type="cellIs" dxfId="208" priority="188" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="207" priority="189" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="190" priority="187" operator="equal">
+    <cfRule type="cellIs" dxfId="206" priority="187" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="189" priority="191" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="192" operator="equal">
+    <cfRule type="cellIs" dxfId="205" priority="191" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="204" priority="192" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I10">
-    <cfRule type="cellIs" dxfId="187" priority="190" operator="equal">
+    <cfRule type="cellIs" dxfId="203" priority="190" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="186" priority="182" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="185" priority="183" operator="equal">
+    <cfRule type="cellIs" dxfId="202" priority="182" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="201" priority="183" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="184" priority="181" operator="equal">
+    <cfRule type="cellIs" dxfId="200" priority="181" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="183" priority="185" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="182" priority="186" operator="equal">
+    <cfRule type="cellIs" dxfId="199" priority="185" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="198" priority="186" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I11">
-    <cfRule type="cellIs" dxfId="181" priority="184" operator="equal">
+    <cfRule type="cellIs" dxfId="197" priority="184" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="180" priority="176" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="179" priority="177" operator="equal">
+    <cfRule type="cellIs" dxfId="196" priority="176" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="195" priority="177" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="178" priority="175" operator="equal">
+    <cfRule type="cellIs" dxfId="194" priority="175" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="177" priority="179" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="176" priority="180" operator="equal">
+    <cfRule type="cellIs" dxfId="193" priority="179" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="192" priority="180" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I12">
-    <cfRule type="cellIs" dxfId="175" priority="178" operator="equal">
+    <cfRule type="cellIs" dxfId="191" priority="178" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="174" priority="170" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="173" priority="171" operator="equal">
+    <cfRule type="cellIs" dxfId="190" priority="170" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="189" priority="171" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="172" priority="169" operator="equal">
+    <cfRule type="cellIs" dxfId="188" priority="169" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="171" priority="173" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="174" operator="equal">
+    <cfRule type="cellIs" dxfId="187" priority="173" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="186" priority="174" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I13">
-    <cfRule type="cellIs" dxfId="169" priority="172" operator="equal">
+    <cfRule type="cellIs" dxfId="185" priority="172" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="168" priority="164" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="167" priority="165" operator="equal">
+    <cfRule type="cellIs" dxfId="184" priority="164" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="183" priority="165" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="166" priority="163" operator="equal">
+    <cfRule type="cellIs" dxfId="182" priority="163" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="165" priority="167" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="164" priority="168" operator="equal">
+    <cfRule type="cellIs" dxfId="181" priority="167" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="180" priority="168" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="cellIs" dxfId="163" priority="166" operator="equal">
+    <cfRule type="cellIs" dxfId="179" priority="166" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="162" priority="158" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="161" priority="159" operator="equal">
+    <cfRule type="cellIs" dxfId="178" priority="158" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="177" priority="159" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="160" priority="157" operator="equal">
+    <cfRule type="cellIs" dxfId="176" priority="157" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="159" priority="161" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="158" priority="162" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="161" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="174" priority="162" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I15">
-    <cfRule type="cellIs" dxfId="157" priority="160" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="160" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="156" priority="152" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="153" operator="equal">
+    <cfRule type="cellIs" dxfId="172" priority="152" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="171" priority="153" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="154" priority="151" operator="equal">
+    <cfRule type="cellIs" dxfId="170" priority="151" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="153" priority="155" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="152" priority="156" operator="equal">
+    <cfRule type="cellIs" dxfId="169" priority="155" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="168" priority="156" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="cellIs" dxfId="151" priority="154" operator="equal">
+    <cfRule type="cellIs" dxfId="167" priority="154" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="150" priority="149" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="150" operator="equal">
+    <cfRule type="cellIs" dxfId="166" priority="149" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="165" priority="150" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="148" priority="148" operator="equal">
+    <cfRule type="cellIs" dxfId="164" priority="148" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="147" priority="146" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="146" priority="147" operator="equal">
+    <cfRule type="cellIs" dxfId="163" priority="146" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="162" priority="147" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5">
-    <cfRule type="cellIs" dxfId="145" priority="145" operator="equal">
+    <cfRule type="cellIs" dxfId="161" priority="145" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="144" priority="50" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="143" priority="51" operator="equal">
+    <cfRule type="cellIs" dxfId="160" priority="50" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="159" priority="51" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="142" priority="49" operator="equal">
+    <cfRule type="cellIs" dxfId="158" priority="49" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="cellIs" dxfId="141" priority="71" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="140" priority="72" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="71" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="156" priority="72" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="cellIs" dxfId="139" priority="70" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="70" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="cellIs" dxfId="138" priority="68" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="137" priority="69" operator="equal">
+    <cfRule type="cellIs" dxfId="154" priority="68" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="153" priority="69" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M6">
-    <cfRule type="cellIs" dxfId="136" priority="67" operator="equal">
+    <cfRule type="cellIs" dxfId="152" priority="67" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="135" priority="62" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="151" priority="62" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="150" priority="63" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="133" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="61" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="132" priority="65" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="131" priority="66" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="65" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="147" priority="66" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7">
-    <cfRule type="cellIs" dxfId="130" priority="64" operator="equal">
+    <cfRule type="cellIs" dxfId="146" priority="64" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="129" priority="56" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="128" priority="57" operator="equal">
+    <cfRule type="cellIs" dxfId="145" priority="56" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="144" priority="57" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="127" priority="55" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="55" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="126" priority="59" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="125" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="59" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="141" priority="60" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M8">
-    <cfRule type="cellIs" dxfId="124" priority="58" operator="equal">
+    <cfRule type="cellIs" dxfId="140" priority="58" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="123" priority="53" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="122" priority="54" operator="equal">
+    <cfRule type="cellIs" dxfId="139" priority="53" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="138" priority="54" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9">
-    <cfRule type="cellIs" dxfId="121" priority="52" operator="equal">
+    <cfRule type="cellIs" dxfId="137" priority="52" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="120" priority="44" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="119" priority="45" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="44" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="135" priority="45" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="118" priority="43" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="43" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="117" priority="47" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="133" priority="47" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="132" priority="48" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M10">
-    <cfRule type="cellIs" dxfId="115" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="131" priority="46" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="114" priority="38" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="113" priority="39" operator="equal">
+    <cfRule type="cellIs" dxfId="130" priority="38" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="129" priority="39" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="112" priority="37" operator="equal">
+    <cfRule type="cellIs" dxfId="128" priority="37" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="111" priority="41" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="110" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="127" priority="41" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="126" priority="42" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M11">
-    <cfRule type="cellIs" dxfId="109" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="125" priority="40" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="108" priority="32" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="107" priority="33" operator="equal">
+    <cfRule type="cellIs" dxfId="124" priority="32" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="123" priority="33" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="106" priority="31" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="31" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="105" priority="35" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="36" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="35" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="120" priority="36" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M12">
-    <cfRule type="cellIs" dxfId="103" priority="34" operator="equal">
+    <cfRule type="cellIs" dxfId="119" priority="34" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="102" priority="26" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="118" priority="26" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="117" priority="27" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="100" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="116" priority="25" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="99" priority="29" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="98" priority="30" operator="equal">
+    <cfRule type="cellIs" dxfId="115" priority="29" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="114" priority="30" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M13">
-    <cfRule type="cellIs" dxfId="97" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="113" priority="28" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="96" priority="20" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="95" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="112" priority="20" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="111" priority="21" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="94" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="110" priority="19" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="93" priority="23" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="92" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="109" priority="23" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="108" priority="24" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M14">
-    <cfRule type="cellIs" dxfId="91" priority="22" operator="equal">
+    <cfRule type="cellIs" dxfId="107" priority="22" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="90" priority="14" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="89" priority="15" operator="equal">
+    <cfRule type="cellIs" dxfId="106" priority="14" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="15" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="88" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="104" priority="13" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="87" priority="17" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="86" priority="18" operator="equal">
+    <cfRule type="cellIs" dxfId="103" priority="17" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="102" priority="18" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M15">
-    <cfRule type="cellIs" dxfId="85" priority="16" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="16" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="84" priority="8" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="8" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="9" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="82" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="98" priority="7" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="81" priority="11" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="80" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="97" priority="11" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="96" priority="12" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M16">
-    <cfRule type="cellIs" dxfId="79" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="95" priority="10" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="78" priority="5" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="77" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="94" priority="5" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="6" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="76" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="92" priority="4" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="75" priority="2" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="74" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="91" priority="2" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="90" priority="3" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5">
-    <cfRule type="cellIs" dxfId="73" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="1" operator="equal">
       <formula>"Please try again"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5196,180 +5406,208 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:K32"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F3"/>
+      <selection activeCell="B3" sqref="B3:B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="10.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.77734375" customWidth="1"/>
     <col min="3" max="3" width="23.5546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="2.109375" customWidth="1"/>
     <col min="5" max="5" width="21.44140625" style="57" customWidth="1"/>
     <col min="6" max="6" width="15.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A1" s="61" t="str">
-        <f>[1]!wwsSetup("useHTTPS", TRUE)</f>
-        <v>useHTTPS = "True"</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="34.200000000000003" x14ac:dyDescent="0.8">
-      <c r="A2" s="66" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="66"/>
-      <c r="C2" s="66"/>
-      <c r="D2" s="11"/>
-      <c r="E2" s="8"/>
-      <c r="F2" s="18"/>
-    </row>
-    <row r="3" spans="1:13" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="67" t="str">
-        <f>CONCATENATE("©ESLatHoward.com"," ","2/6/20")</f>
-        <v>©ESLatHoward.com 2/6/20</v>
-      </c>
-      <c r="B3" s="67"/>
-      <c r="C3" s="67"/>
-      <c r="D3" s="67"/>
-      <c r="E3" s="67"/>
-      <c r="F3" s="67"/>
-    </row>
-    <row r="4" spans="1:13" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="A4" s="23"/>
-      <c r="B4" s="26"/>
-      <c r="C4" s="40"/>
-      <c r="E4" s="64" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
+    <row r="1" spans="1:11" ht="31.2" x14ac:dyDescent="0.35">
+      <c r="A1" s="67" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="67"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="69" t="s">
+        <v>66</v>
+      </c>
+      <c r="G1" s="70"/>
+      <c r="H1" s="70"/>
+      <c r="I1" s="70"/>
+      <c r="J1" s="71"/>
+      <c r="K1" s="70"/>
+    </row>
+    <row r="2" spans="1:11" ht="27.6" x14ac:dyDescent="0.35">
+      <c r="A2" s="72" t="s">
+        <v>67</v>
+      </c>
+      <c r="B2" s="72"/>
+      <c r="C2" s="72"/>
+      <c r="D2" s="72"/>
+      <c r="E2" s="72"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="70"/>
+    </row>
+    <row r="3" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.7">
+      <c r="B3" s="74" t="str">
+        <f>[1]!wwsImage("Janice.jpg",120,160)</f>
+        <v/>
+      </c>
+      <c r="C3" s="40"/>
+      <c r="E3" s="63" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A4" s="75"/>
+      <c r="B4" s="74"/>
+      <c r="C4" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="58" t="str">
+        <f>[1]!wwsInput()</f>
+        <v/>
+      </c>
+      <c r="F4" s="18" t="str">
+        <f>IF(E4&lt;&gt;"",IF(EXACT(TRIM(E4),TRIM(C4)),"GOOD",IF(E4="sunday","S?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A5" s="75"/>
+      <c r="B5" s="74"/>
       <c r="C5" s="39" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="21"/>
-      <c r="E5" s="58" t="str">
+      <c r="E5" s="59" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F5" s="18" t="str">
-        <f>IF(E5&lt;&gt;"",IF(EXACT(TRIM(E5),TRIM(C5)),"GOOD",IF(E5="sunday","S?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B6" s="21"/>
+        <f>IF(E5&lt;&gt;"",IF(EXACT(TRIM(E5),TRIM(C5)),"GOOD",IF(E5="monday","M?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G5" s="18"/>
+    </row>
+    <row r="6" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A6" s="75"/>
+      <c r="B6" s="74"/>
       <c r="C6" s="39" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="21"/>
-      <c r="E6" s="59" t="str">
+        <v>14</v>
+      </c>
+      <c r="D6" s="30"/>
+      <c r="E6" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F6" s="18" t="str">
-        <f>IF(E6&lt;&gt;"",IF(EXACT(TRIM(E6),TRIM(C6)),"GOOD",IF(E6="monday","M?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G6" s="18"/>
-    </row>
-    <row r="7" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B7" s="29"/>
+        <f>IF(E6&lt;&gt;"",IF(EXACT(TRIM(E6),TRIM(C6)),"GOOD",IF(E6="tuesday","T?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G6" s="31"/>
+    </row>
+    <row r="7" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A7" s="65"/>
+      <c r="B7" s="74"/>
       <c r="C7" s="39" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="30"/>
+        <v>15</v>
+      </c>
+      <c r="D7" s="21"/>
       <c r="E7" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F7" s="18" t="str">
-        <f>IF(E7&lt;&gt;"",IF(EXACT(TRIM(E7),TRIM(C7)),"GOOD",IF(E7="tuesday","T?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G7" s="31"/>
-    </row>
-    <row r="8" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B8" s="21"/>
+        <f>IF(E7&lt;&gt;"",IF(EXACT(TRIM(E7),TRIM(C7)),"GOOD",IF(E7="wednesday","W?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G7" s="18"/>
+    </row>
+    <row r="8" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="A8" s="23"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="39" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="21"/>
+        <v>16</v>
+      </c>
+      <c r="D8" s="30"/>
       <c r="E8" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F8" s="18" t="str">
-        <f>IF(E8&lt;&gt;"",IF(EXACT(TRIM(E8),TRIM(C8)),"GOOD",IF(E8="wednesday","W?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G8" s="18"/>
-    </row>
-    <row r="9" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
-      <c r="B9" s="29"/>
+        <f>IF(E8&lt;&gt;"",IF(EXACT(TRIM(E8),TRIM(C8)),"GOOD",IF(E8="thursday","T?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G8" s="31"/>
+    </row>
+    <row r="9" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="C9" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="D9" s="30"/>
+        <v>17</v>
+      </c>
+      <c r="D9" s="21"/>
       <c r="E9" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F9" s="18" t="str">
-        <f>IF(E9&lt;&gt;"",IF(EXACT(TRIM(E9),TRIM(C9)),"GOOD",IF(E9="thursday","T?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G9" s="31"/>
-    </row>
-    <row r="10" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
+        <f>IF(E9&lt;&gt;"",IF(EXACT(TRIM(E9),TRIM(C9)),"GOOD",IF(E9="friday","F?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G9" s="18"/>
+    </row>
+    <row r="10" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B10" s="21"/>
       <c r="C10" s="39" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="21"/>
+        <v>18</v>
+      </c>
+      <c r="D10" s="30"/>
       <c r="E10" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F10" s="18" t="str">
-        <f>IF(E10&lt;&gt;"",IF(EXACT(TRIM(E10),TRIM(C10)),"GOOD",IF(E10="friday","F?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G10" s="18"/>
-      <c r="M10" s="38"/>
-    </row>
-    <row r="11" spans="1:13" ht="31.95" customHeight="1" x14ac:dyDescent="0.8">
+        <f>IF(E10&lt;&gt;"",IF(EXACT(TRIM(E10),TRIM(C10)),"GOOD",IF(E10="saturday","S?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G10" s="31"/>
+    </row>
+    <row r="11" spans="1:11" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B11" s="29"/>
-      <c r="C11" s="39" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="30"/>
-      <c r="E11" s="60" t="str">
+      <c r="C11" s="61" t="s">
+        <v>68</v>
+      </c>
+      <c r="D11" s="38"/>
+      <c r="E11" s="62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B12" s="21"/>
+      <c r="C12" s="39" t="s">
+        <v>51</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
-      <c r="F11" s="18" t="str">
-        <f>IF(E11&lt;&gt;"",IF(EXACT(TRIM(E11),TRIM(C11)),"GOOD",IF(E11="saturday","S?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G11" s="31"/>
-    </row>
-    <row r="12" spans="1:13" ht="58.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="B12" s="21"/>
-      <c r="C12" s="62" t="s">
-        <v>24</v>
-      </c>
-      <c r="D12" s="38"/>
-      <c r="E12" s="63" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="34.200000000000003" x14ac:dyDescent="0.8">
+      <c r="F12" s="18" t="str">
+        <f>IF(E12&lt;&gt;"",IF(EXACT(TRIM(E12),TRIM(C4)),"GOOD",IF(E12="sunday","S?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G12" s="31"/>
+    </row>
+    <row r="13" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B13" s="21"/>
       <c r="C13" s="39" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D13" s="21"/>
       <c r="E13" s="58" t="str">
@@ -5377,47 +5615,47 @@
         <v/>
       </c>
       <c r="F13" s="18" t="str">
-        <f>IF(E13&lt;&gt;"",IF(EXACT(TRIM(E13),TRIM(C5)),"GOOD",IF(E13="sunday","S?","?"))," ")</f>
+        <f>IF(E13&lt;&gt;"",IF(EXACT(TRIM(E13),TRIM(C5)),"GOOD",IF(E13="monday","M?","?"))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G13" s="31"/>
     </row>
-    <row r="14" spans="1:13" ht="34.200000000000003" x14ac:dyDescent="0.8">
+    <row r="14" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B14" s="21"/>
       <c r="C14" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D14" s="21"/>
+      <c r="E14" s="58" t="str">
+        <f>[1]!wwsInput()</f>
+        <v/>
+      </c>
+      <c r="F14" s="18" t="str">
+        <f>IF(E14&lt;&gt;"",IF(EXACT(TRIM(E14),TRIM(C6)),"GOOD",IF(E14="tuesday","T?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G14" s="31"/>
+    </row>
+    <row r="15" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B15" s="21"/>
+      <c r="C15" s="39" t="s">
         <v>54</v>
       </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="59" t="str">
-        <f>[1]!wwsInput()</f>
-        <v/>
-      </c>
-      <c r="F14" s="18" t="str">
-        <f>IF(E14&lt;&gt;"",IF(EXACT(TRIM(E14),TRIM(C6)),"GOOD",IF(E14="monday","M?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G14" s="18"/>
-    </row>
-    <row r="15" spans="1:13" ht="34.200000000000003" x14ac:dyDescent="0.8">
-      <c r="B15" s="29"/>
-      <c r="C15" s="39" t="s">
-        <v>55</v>
-      </c>
-      <c r="D15" s="30"/>
+      <c r="D15" s="21"/>
       <c r="E15" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F15" s="18" t="str">
-        <f>IF(E15&lt;&gt;"",IF(EXACT(TRIM(E15),TRIM(C7)),"GOOD",IF(E15="tuesday","T?","?"))," ")</f>
+        <f>IF(E15&lt;&gt;"",IF(EXACT(TRIM(E15),TRIM(C7)),"GOOD",IF(E15="wednesday","W?","?"))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G15" s="31"/>
     </row>
-    <row r="16" spans="1:13" ht="34.200000000000003" x14ac:dyDescent="0.8">
+    <row r="16" spans="1:11" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B16" s="21"/>
       <c r="C16" s="39" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D16" s="21"/>
       <c r="E16" s="58" t="str">
@@ -5425,31 +5663,31 @@
         <v/>
       </c>
       <c r="F16" s="18" t="str">
-        <f>IF(E16&lt;&gt;"",IF(EXACT(TRIM(E16),TRIM(C8)),"GOOD",IF(E16="wednesday","W?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="G16" s="18"/>
-    </row>
-    <row r="17" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
-      <c r="B17" s="29"/>
+        <f>IF(E16&lt;&gt;"",IF(EXACT(TRIM(E16),TRIM(C8)),"GOOD",IF(E16="thursday","T?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G16" s="31"/>
+    </row>
+    <row r="17" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B17" s="21"/>
       <c r="C17" s="39" t="s">
-        <v>57</v>
-      </c>
-      <c r="D17" s="30"/>
+        <v>56</v>
+      </c>
+      <c r="D17" s="21"/>
       <c r="E17" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F17" s="18" t="str">
-        <f>IF(E17&lt;&gt;"",IF(EXACT(TRIM(E17),TRIM(C9)),"GOOD",IF(E17="thursday","T?","?"))," ")</f>
+        <f>IF(E17&lt;&gt;"",IF(EXACT(TRIM(E17),TRIM(C9)),"GOOD",IF(E17="friday","F?","?"))," ")</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="G17" s="31"/>
     </row>
-    <row r="18" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+    <row r="18" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B18" s="21"/>
       <c r="C18" s="39" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D18" s="21"/>
       <c r="E18" s="58" t="str">
@@ -5457,81 +5695,85 @@
         <v/>
       </c>
       <c r="F18" s="18" t="str">
-        <f>IF(E18&lt;&gt;"",IF(EXACT(TRIM(E18),TRIM(C10)),"GOOD",IF(E18="friday","F?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="19" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+        <f>IF(E18&lt;&gt;"",IF(EXACT(TRIM(E18),TRIM(C10)),"GOOD",IF(E18="saturday","S?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="G18" s="31"/>
+    </row>
+    <row r="19" spans="2:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.7">
       <c r="B19" s="29"/>
-      <c r="C19" s="39" t="s">
+      <c r="C19" s="61" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="38"/>
+      <c r="E19" s="62" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B20" s="21"/>
+      <c r="C20" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="58" t="str">
+        <f>[1]!wwsInput()</f>
+        <v/>
+      </c>
+      <c r="F20" s="18" t="str">
+        <f>IF(E20&lt;&gt;"",IF(EXACT(TRIM(E20),TRIM(C4)),"GOOD",IF(E20="sunday","S?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B21" s="29"/>
+      <c r="C21" s="39" t="s">
         <v>59</v>
       </c>
-      <c r="D19" s="30"/>
-      <c r="E19" s="60" t="str">
+      <c r="D21" s="21"/>
+      <c r="E21" s="59" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
-      <c r="F19" s="18" t="str">
-        <f>IF(E19&lt;&gt;"",IF(EXACT(TRIM(E19),TRIM(C11)),"GOOD",IF(E19="saturday","S?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="20" spans="2:7" ht="58.8" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="C20" s="62" t="s">
-        <v>23</v>
-      </c>
-      <c r="E20" s="63" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="21" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
-      <c r="C21" s="39" t="s">
-        <v>60</v>
-      </c>
-      <c r="D21" s="21"/>
-      <c r="E21" s="58" t="str">
-        <f>[1]!wwsInput()</f>
-        <v/>
-      </c>
       <c r="F21" s="18" t="str">
-        <f>IF(E21&lt;&gt;"",IF(EXACT(TRIM(E21),TRIM(C5)),"GOOD",IF(E21="sunday","S?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="22" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+        <f>IF(E21&lt;&gt;"",IF(EXACT(TRIM(E21),TRIM(C5)),"GOOD",IF(E21="monday","M?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B22" s="21"/>
       <c r="C22" s="39" t="s">
-        <v>61</v>
-      </c>
-      <c r="D22" s="21"/>
-      <c r="E22" s="59" t="str">
+        <v>60</v>
+      </c>
+      <c r="D22" s="30"/>
+      <c r="E22" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F22" s="18" t="str">
-        <f>IF(E22&lt;&gt;"",IF(EXACT(TRIM(E22),TRIM(C6)),"GOOD",IF(E22="monday","M?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="23" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+        <f>IF(E22&lt;&gt;"",IF(EXACT(TRIM(E22),TRIM(C6)),"GOOD",IF(E22="tuesday","T?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B23" s="29"/>
       <c r="C23" s="39" t="s">
-        <v>62</v>
-      </c>
-      <c r="D23" s="30"/>
+        <v>61</v>
+      </c>
+      <c r="D23" s="21"/>
       <c r="E23" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F23" s="18" t="str">
-        <f>IF(E23&lt;&gt;"",IF(EXACT(TRIM(E23),TRIM(C7)),"GOOD",IF(E23="tuesday","T?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="24" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+        <f>IF(E23&lt;&gt;"",IF(EXACT(TRIM(E23),TRIM(C7)),"GOOD",IF(E23="wednesday","W?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B24" s="21"/>
       <c r="C24" s="39" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="21"/>
       <c r="E24" s="58" t="str">
@@ -5539,29 +5781,29 @@
         <v/>
       </c>
       <c r="F24" s="18" t="str">
-        <f>IF(E24&lt;&gt;"",IF(EXACT(TRIM(E24),TRIM(C8)),"GOOD",IF(E24="wednesday","W?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="25" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
-      <c r="B25" s="29"/>
+        <f>IF(E24&lt;&gt;"",IF(EXACT(TRIM(E24),TRIM(C8)),"GOOD",IF(E24="thursday","T?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
+      <c r="B25" s="21"/>
       <c r="C25" s="39" t="s">
-        <v>64</v>
-      </c>
-      <c r="D25" s="30"/>
+        <v>63</v>
+      </c>
+      <c r="D25" s="21"/>
       <c r="E25" s="58" t="str">
         <f>[1]!wwsInput()</f>
         <v/>
       </c>
       <c r="F25" s="18" t="str">
-        <f>IF(E25&lt;&gt;"",IF(EXACT(TRIM(E25),TRIM(C9)),"GOOD",IF(E25="thursday","T?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="26" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+        <f>IF(E25&lt;&gt;"",IF(EXACT(TRIM(E25),TRIM(C9)),"GOOD",IF(E25="friday","F?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" ht="28.8" customHeight="1" x14ac:dyDescent="0.8">
       <c r="B26" s="21"/>
       <c r="C26" s="39" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D26" s="21"/>
       <c r="E26" s="58" t="str">
@@ -5569,214 +5811,207 @@
         <v/>
       </c>
       <c r="F26" s="18" t="str">
-        <f>IF(E26&lt;&gt;"",IF(EXACT(TRIM(E26),TRIM(C10)),"GOOD",IF(E26="friday","F?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="27" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+        <f>IF(E26&lt;&gt;"",IF(EXACT(TRIM(E26),TRIM(C10)),"GOOD",IF(E26="saturday","S?","?"))," ")</f>
+        <v xml:space="preserve"> </v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" ht="30" x14ac:dyDescent="0.7">
       <c r="B27" s="29"/>
-      <c r="C27" s="39" t="s">
-        <v>66</v>
-      </c>
-      <c r="D27" s="30"/>
-      <c r="E27" s="60" t="str">
-        <f>[1]!wwsInput()</f>
-        <v/>
-      </c>
-      <c r="F27" s="18" t="str">
-        <f>IF(E27&lt;&gt;"",IF(EXACT(TRIM(E27),TRIM(C11)),"GOOD",IF(E27="saturday","S?","?"))," ")</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="28" spans="2:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="G28" s="38" t="s">
+      <c r="G27" s="38" t="s">
         <v>21</v>
       </c>
     </row>
+    <row r="28" spans="2:7" ht="30" x14ac:dyDescent="0.7">
+      <c r="B28" s="21"/>
+    </row>
+    <row r="29" spans="2:7" ht="30" x14ac:dyDescent="0.7">
+      <c r="B29" s="29"/>
+    </row>
+    <row r="30" spans="2:7" ht="30" x14ac:dyDescent="0.7">
+      <c r="B30" s="21"/>
+    </row>
+    <row r="31" spans="2:7" ht="34.200000000000003" x14ac:dyDescent="0.8">
+      <c r="B31" s="29"/>
+    </row>
+    <row r="32" spans="2:7" ht="26.4" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <sheetProtection selectLockedCells="1"/>
-  <mergeCells count="2">
-    <mergeCell ref="A2:C2"/>
-    <mergeCell ref="A3:F3"/>
+  <mergeCells count="3">
+    <mergeCell ref="B3:B7"/>
+    <mergeCell ref="A2:E2"/>
+    <mergeCell ref="A1:B1"/>
   </mergeCells>
-  <conditionalFormatting sqref="F2">
-    <cfRule type="cellIs" dxfId="72" priority="106" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="107" operator="equal">
+  <conditionalFormatting sqref="F4">
+    <cfRule type="cellIs" dxfId="80" priority="103" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="79" priority="104" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="78" priority="101" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="77" priority="102" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6">
+    <cfRule type="cellIs" dxfId="76" priority="99" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="75" priority="100" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F7">
+    <cfRule type="cellIs" dxfId="74" priority="97" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="73" priority="98" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F8">
+    <cfRule type="cellIs" dxfId="72" priority="95" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="71" priority="96" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F9">
+    <cfRule type="cellIs" dxfId="70" priority="93" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="69" priority="94" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F10">
+    <cfRule type="cellIs" dxfId="68" priority="91" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="67" priority="92" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F13">
+    <cfRule type="cellIs" dxfId="64" priority="17" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="63" priority="18" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F12">
+    <cfRule type="cellIs" dxfId="62" priority="59" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="61" priority="60" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F18">
+    <cfRule type="cellIs" dxfId="58" priority="5" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="57" priority="6" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F22">
+    <cfRule type="cellIs" dxfId="56" priority="29" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="55" priority="30" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="cellIs" dxfId="54" priority="27" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="53" priority="28" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16">
+    <cfRule type="cellIs" dxfId="52" priority="9" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="51" priority="10" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F17">
+    <cfRule type="cellIs" dxfId="50" priority="7" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="49" priority="8" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F20">
+    <cfRule type="cellIs" dxfId="48" priority="33" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="47" priority="34" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F21">
+    <cfRule type="cellIs" dxfId="46" priority="31" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="45" priority="32" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="cellIs" dxfId="42" priority="15" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="41" priority="16" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F14">
+    <cfRule type="cellIs" dxfId="40" priority="13" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="39" priority="14" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F15">
-    <cfRule type="cellIs" dxfId="70" priority="25" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="26" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F16">
-    <cfRule type="cellIs" dxfId="68" priority="23" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="24" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F17">
-    <cfRule type="cellIs" dxfId="66" priority="21" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="22" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F5">
-    <cfRule type="cellIs" dxfId="64" priority="85" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="86" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F6">
-    <cfRule type="cellIs" dxfId="62" priority="83" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="84" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F7">
-    <cfRule type="cellIs" dxfId="60" priority="81" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="82" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F8">
-    <cfRule type="cellIs" dxfId="58" priority="79" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="80" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F9">
-    <cfRule type="cellIs" dxfId="56" priority="77" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="55" priority="78" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F10">
-    <cfRule type="cellIs" dxfId="54" priority="75" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="76" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F11">
-    <cfRule type="cellIs" dxfId="52" priority="73" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="51" priority="74" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F18">
-    <cfRule type="cellIs" dxfId="50" priority="19" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="20" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F19">
-    <cfRule type="cellIs" dxfId="48" priority="17" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="47" priority="18" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F13">
-    <cfRule type="cellIs" dxfId="46" priority="41" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="45" priority="42" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F14">
-    <cfRule type="cellIs" dxfId="44" priority="37" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="43" priority="38" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
-    <cfRule type="cellIs" dxfId="42" priority="3" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="41" priority="4" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F23">
-    <cfRule type="cellIs" dxfId="40" priority="11" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="39" priority="12" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F24">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="38" priority="11" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="37" priority="12" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F25">
-    <cfRule type="cellIs" dxfId="36" priority="7" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="35" priority="8" operator="equal">
+    <cfRule type="cellIs" dxfId="30" priority="3" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="29" priority="4" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F26">
-    <cfRule type="cellIs" dxfId="34" priority="5" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="33" priority="6" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F21">
-    <cfRule type="cellIs" dxfId="32" priority="15" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="31" priority="16" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F22">
-    <cfRule type="cellIs" dxfId="30" priority="13" operator="equal">
-      <formula>"Correct!"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="29" priority="14" operator="equal">
+    <cfRule type="cellIs" dxfId="28" priority="1" operator="equal">
+      <formula>"Correct!"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="27" priority="2" operator="equal">
       <formula>"Correct!"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5801,7 +6036,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="9.6" customHeight="1" x14ac:dyDescent="0.7">
-      <c r="A1" s="61" t="str">
+      <c r="A1" s="60" t="str">
         <f>[1]!wwsSetup("useHTTPS", TRUE)</f>
         <v>useHTTPS = "True"</v>
       </c>
@@ -6547,7 +6782,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.8">
-      <c r="A1" s="61" t="str">
+      <c r="A1" s="60" t="str">
         <f>[1]!wwsSetup("useHTTPS", TRUE)</f>
         <v>useHTTPS = "True"</v>
       </c>

</xml_diff>